<commit_message>
Calculating and visualizing additional experimental data Tygstrup
</commit_message>
<xml_diff>
--- a/experimental_data/GEC/Tygstrup1958.xlsx
+++ b/experimental_data/GEC/Tygstrup1958.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="103">
   <si>
     <t>Tygstrup1958 – Galactose blood clearance as a measure of hepatic blood flow</t>
   </si>
@@ -71,9 +71,18 @@
     <t>Arterial blood galactose [mg/100ml]</t>
   </si>
   <si>
+    <t>Galactose extraction fraction [-]</t>
+  </si>
+  <si>
     <t>Arterial blood galactose [mmole/l]</t>
   </si>
   <si>
+    <t>Venous blood galactose via cv = (1-ER)*ca [mmole/l]</t>
+  </si>
+  <si>
+    <t>Galactose elimination rate [mmole/min]</t>
+  </si>
+  <si>
     <t>study</t>
   </si>
   <si>
@@ -101,10 +110,10 @@
     <t>diagnosis</t>
   </si>
   <si>
-    <t>galclearance</t>
-  </si>
-  <si>
-    <t>extraction</t>
+    <t>CL</t>
+  </si>
+  <si>
+    <t>ER100</t>
   </si>
   <si>
     <t>bloodflowBS</t>
@@ -113,7 +122,7 @@
     <t>bloodFlowGal</t>
   </si>
   <si>
-    <t>clFraction</t>
+    <t>CLFraction</t>
   </si>
   <si>
     <t>infusionRatemg</t>
@@ -122,10 +131,19 @@
     <t>infusionRate</t>
   </si>
   <si>
-    <t>galAmg</t>
-  </si>
-  <si>
-    <t>galA</t>
+    <t>camg</t>
+  </si>
+  <si>
+    <t>ER</t>
+  </si>
+  <si>
+    <t>ca</t>
+  </si>
+  <si>
+    <t>cv</t>
+  </si>
+  <si>
+    <t>GE</t>
   </si>
   <si>
     <t>tyg1958</t>
@@ -539,16 +557,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>804960</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>71640</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>46080</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>128880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>337680</xdr:colOff>
-      <xdr:row>83</xdr:row>
-      <xdr:rowOff>65160</xdr:rowOff>
+      <xdr:colOff>390960</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>35280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -563,8 +581,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5476320" y="9124200"/>
-          <a:ext cx="5273280" cy="4296240"/>
+          <a:off x="5530320" y="9106200"/>
+          <a:ext cx="5272560" cy="4295520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -579,15 +597,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>348480</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>97920</xdr:rowOff>
+      <xdr:colOff>402480</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>155160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>651240</xdr:colOff>
-      <xdr:row>80</xdr:row>
-      <xdr:rowOff>82080</xdr:rowOff>
+      <xdr:colOff>704520</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>78480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -602,8 +620,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="348480" y="9150480"/>
-          <a:ext cx="4974120" cy="3825720"/>
+          <a:off x="402480" y="9132480"/>
+          <a:ext cx="4973400" cy="3825000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -617,16 +635,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>459720</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>59040</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>542880</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>3600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>736560</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>41040</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>6120</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>108360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -635,8 +653,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15748560" y="212400"/>
-          <a:ext cx="5966280" cy="2580480"/>
+          <a:off x="17457120" y="328680"/>
+          <a:ext cx="5965560" cy="2579760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -683,16 +701,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>561240</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>665280</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>119520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>675360</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>96840</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>778680</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>17640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -707,8 +725,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15037200" y="6324480"/>
-          <a:ext cx="4991040" cy="2824920"/>
+          <a:off x="13515480" y="7796520"/>
+          <a:ext cx="4990320" cy="2824200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -728,13 +746,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R38"/>
+  <dimension ref="A1:U38"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R38" activeCellId="0" sqref="A4:R38"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U37" activeCellId="0" sqref="U37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.1"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.61224489795918"/>
@@ -743,7 +761,7 @@
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -754,10 +772,10 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="3"/>
     </row>
-    <row r="3" s="5" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="5" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -812,75 +830,93 @@
       <c r="R3" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="S3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="R4" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
+      </c>
+      <c r="S4" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="U4" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B5" s="7" t="n">
         <v>1</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E5" s="7" t="n">
         <v>20</v>
@@ -892,25 +928,25 @@
         <v>1.88</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="J5" s="7" t="n">
         <v>1010</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="O5" s="7" t="n">
         <v>267</v>
@@ -922,23 +958,32 @@
       <c r="Q5" s="7" t="n">
         <v>26.5</v>
       </c>
-      <c r="R5" s="7" t="n">
+      <c r="R5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="S5" s="7" t="n">
         <f aca="false">Q5/18</f>
         <v>1.47222222222222</v>
       </c>
+      <c r="T5" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="U5" s="0" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B6" s="7" t="n">
         <v>2</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E6" s="7" t="n">
         <v>23</v>
@@ -950,25 +995,25 @@
         <v>1.76</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="J6" s="7" t="n">
         <v>1020</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="O6" s="7" t="n">
         <v>309</v>
@@ -980,23 +1025,32 @@
       <c r="Q6" s="7" t="n">
         <v>30.2</v>
       </c>
-      <c r="R6" s="7" t="n">
+      <c r="R6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="S6" s="7" t="n">
         <f aca="false">Q6/18</f>
         <v>1.67777777777778</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T6" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="U6" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B7" s="7" t="n">
         <v>3</v>
       </c>
       <c r="C7" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>39</v>
       </c>
       <c r="E7" s="7" t="n">
         <v>45</v>
@@ -1008,25 +1062,25 @@
         <v>1.55</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="J7" s="7" t="n">
         <v>1390</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="O7" s="7" t="n">
         <v>273</v>
@@ -1038,23 +1092,32 @@
       <c r="Q7" s="7" t="n">
         <v>19.6</v>
       </c>
-      <c r="R7" s="7" t="n">
+      <c r="R7" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="S7" s="7" t="n">
         <f aca="false">Q7/18</f>
         <v>1.08888888888889</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T7" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="U7" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B8" s="7" t="n">
         <v>4</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E8" s="7" t="n">
         <v>48</v>
@@ -1066,25 +1129,25 @@
         <v>1.77</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J8" s="7" t="n">
         <v>1460</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="O8" s="7" t="n">
         <v>314</v>
@@ -1096,23 +1159,32 @@
       <c r="Q8" s="7" t="n">
         <v>21.5</v>
       </c>
-      <c r="R8" s="7" t="n">
+      <c r="R8" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="S8" s="7" t="n">
         <f aca="false">Q8/18</f>
         <v>1.19444444444444</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T8" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="U8" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B9" s="7" t="n">
         <v>5</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E9" s="7" t="n">
         <v>19</v>
@@ -1124,25 +1196,25 @@
         <v>1.8</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="J9" s="7" t="n">
         <v>1310</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="O9" s="7" t="n">
         <v>242</v>
@@ -1154,23 +1226,32 @@
       <c r="Q9" s="7" t="n">
         <v>18.4</v>
       </c>
-      <c r="R9" s="7" t="n">
+      <c r="R9" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="S9" s="7" t="n">
         <f aca="false">Q9/18</f>
         <v>1.02222222222222</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T9" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="U9" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B10" s="7" t="n">
         <v>6</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E10" s="7" t="n">
         <v>40</v>
@@ -1182,25 +1263,25 @@
         <v>1.8</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="J10" s="7" t="n">
         <v>1460</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="O10" s="7" t="n">
         <v>370</v>
@@ -1212,23 +1293,32 @@
       <c r="Q10" s="7" t="n">
         <v>25.4</v>
       </c>
-      <c r="R10" s="7" t="n">
+      <c r="R10" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="S10" s="7" t="n">
         <f aca="false">Q10/18</f>
         <v>1.41111111111111</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T10" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="U10" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B11" s="7" t="n">
         <v>7</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E11" s="7" t="n">
         <v>50</v>
@@ -1240,25 +1330,25 @@
         <v>2.06</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="J11" s="7" t="n">
         <v>1680</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="O11" s="7" t="n">
         <v>334</v>
@@ -1270,23 +1360,32 @@
       <c r="Q11" s="7" t="n">
         <v>19.9</v>
       </c>
-      <c r="R11" s="7" t="n">
+      <c r="R11" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="S11" s="7" t="n">
         <f aca="false">Q11/18</f>
         <v>1.10555555555556</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T11" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="U11" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B12" s="7" t="n">
         <v>8</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E12" s="7" t="n">
         <v>54</v>
@@ -1298,25 +1397,25 @@
         <v>2.01</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="J12" s="7" t="n">
         <v>1470</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="N12" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="O12" s="7" t="n">
         <v>310</v>
@@ -1328,23 +1427,32 @@
       <c r="Q12" s="7" t="n">
         <v>21.2</v>
       </c>
-      <c r="R12" s="7" t="n">
+      <c r="R12" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="S12" s="7" t="n">
         <f aca="false">Q12/18</f>
         <v>1.17777777777778</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T12" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="U12" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B13" s="7" t="n">
         <v>9</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E13" s="7" t="n">
         <v>35</v>
@@ -1356,10 +1464,10 @@
         <v>1.69</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="J13" s="7" t="n">
         <v>1840</v>
@@ -1368,13 +1476,13 @@
         <v>93</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="N13" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="O13" s="7" t="n">
         <v>217</v>
@@ -1387,22 +1495,33 @@
         <v>11.8</v>
       </c>
       <c r="R13" s="7" t="n">
+        <f aca="false">K13/100</f>
+        <v>0.93</v>
+      </c>
+      <c r="S13" s="7" t="n">
         <f aca="false">Q13/18</f>
         <v>0.655555555555556</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T13" s="0" t="n">
+        <f aca="false">S13*(1-R13)</f>
+        <v>0.0458888888888889</v>
+      </c>
+      <c r="U13" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B14" s="7" t="n">
         <v>10</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E14" s="7" t="n">
         <v>57</v>
@@ -1414,10 +1533,10 @@
         <v>1.69</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="J14" s="7" t="n">
         <v>1710</v>
@@ -1426,13 +1545,13 @@
         <v>86</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="M14" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="N14" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="O14" s="7" t="n">
         <v>294</v>
@@ -1445,22 +1564,33 @@
         <v>17.2</v>
       </c>
       <c r="R14" s="7" t="n">
+        <f aca="false">K14/100</f>
+        <v>0.86</v>
+      </c>
+      <c r="S14" s="7" t="n">
         <f aca="false">Q14/18</f>
         <v>0.955555555555555</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T14" s="0" t="n">
+        <f aca="false">S14*(1-R14)</f>
+        <v>0.133777777777778</v>
+      </c>
+      <c r="U14" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B15" s="7" t="n">
         <v>11</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E15" s="7" t="n">
         <v>14</v>
@@ -1472,10 +1602,10 @@
         <v>1.54</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="J15" s="7" t="n">
         <v>660</v>
@@ -1487,7 +1617,7 @@
         <v>670</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="N15" s="7" t="n">
         <v>0.98</v>
@@ -1503,22 +1633,34 @@
         <v>41.2</v>
       </c>
       <c r="R15" s="7" t="n">
+        <f aca="false">K15/100</f>
+        <v>0.95</v>
+      </c>
+      <c r="S15" s="7" t="n">
         <f aca="false">Q15/18</f>
         <v>2.28888888888889</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T15" s="0" t="n">
+        <f aca="false">S15*(1-R15)</f>
+        <v>0.114444444444445</v>
+      </c>
+      <c r="U15" s="0" t="n">
+        <f aca="false">L15*(S15-T15)/1000</f>
+        <v>1.45687777777778</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B16" s="7" t="n">
         <v>12</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E16" s="7" t="n">
         <v>36</v>
@@ -1530,10 +1672,10 @@
         <v>1.8</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="J16" s="7" t="n">
         <v>1670</v>
@@ -1545,7 +1687,7 @@
         <v>1500</v>
       </c>
       <c r="M16" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="N16" s="7" t="n">
         <v>1.12</v>
@@ -1561,22 +1703,34 @@
         <v>17</v>
       </c>
       <c r="R16" s="7" t="n">
+        <f aca="false">K16/100</f>
+        <v>0.91</v>
+      </c>
+      <c r="S16" s="7" t="n">
         <f aca="false">Q16/18</f>
         <v>0.944444444444444</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T16" s="0" t="n">
+        <f aca="false">S16*(1-R16)</f>
+        <v>0.0849999999999999</v>
+      </c>
+      <c r="U16" s="0" t="n">
+        <f aca="false">L16*(S16-T16)/1000</f>
+        <v>1.28916666666667</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B17" s="7" t="n">
         <v>13</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E17" s="7" t="n">
         <v>47</v>
@@ -1588,10 +1742,10 @@
         <v>1.82</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="J17" s="7" t="n">
         <v>1890</v>
@@ -1603,7 +1757,7 @@
         <v>1630</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="N17" s="7" t="n">
         <v>1.26</v>
@@ -1619,22 +1773,34 @@
         <v>20</v>
       </c>
       <c r="R17" s="7" t="n">
+        <f aca="false">K17/100</f>
+        <v>0.92</v>
+      </c>
+      <c r="S17" s="7" t="n">
         <f aca="false">Q17/18</f>
         <v>1.11111111111111</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T17" s="0" t="n">
+        <f aca="false">S17*(1-R17)</f>
+        <v>0.0888888888888888</v>
+      </c>
+      <c r="U17" s="0" t="n">
+        <f aca="false">L17*(S17-T17)/1000</f>
+        <v>1.66622222222222</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B18" s="7" t="n">
         <v>14</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E18" s="7" t="n">
         <v>19</v>
@@ -1646,10 +1812,10 @@
         <v>1.68</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="J18" s="7" t="n">
         <v>1700</v>
@@ -1661,7 +1827,7 @@
         <v>1280</v>
       </c>
       <c r="M18" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="N18" s="7" t="n">
         <v>1.34</v>
@@ -1677,22 +1843,34 @@
         <v>22.4</v>
       </c>
       <c r="R18" s="7" t="n">
+        <f aca="false">K18/100</f>
+        <v>0.88</v>
+      </c>
+      <c r="S18" s="7" t="n">
         <f aca="false">Q18/18</f>
         <v>1.24444444444444</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T18" s="0" t="n">
+        <f aca="false">S18*(1-R18)</f>
+        <v>0.149333333333333</v>
+      </c>
+      <c r="U18" s="0" t="n">
+        <f aca="false">L18*(S18-T18)/1000</f>
+        <v>1.40174222222222</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B19" s="7" t="n">
         <v>15</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E19" s="7" t="n">
         <v>40</v>
@@ -1704,10 +1882,10 @@
         <v>1.65</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="J19" s="7" t="n">
         <v>1180</v>
@@ -1719,7 +1897,7 @@
         <v>1490</v>
       </c>
       <c r="M19" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="N19" s="7" t="n">
         <v>0.79</v>
@@ -1735,22 +1913,34 @@
         <v>31.4</v>
       </c>
       <c r="R19" s="7" t="n">
+        <f aca="false">K19/100</f>
+        <v>0.73</v>
+      </c>
+      <c r="S19" s="7" t="n">
         <f aca="false">Q19/18</f>
         <v>1.74444444444444</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T19" s="0" t="n">
+        <f aca="false">S19*(1-R19)</f>
+        <v>0.470999999999999</v>
+      </c>
+      <c r="U19" s="0" t="n">
+        <f aca="false">L19*(S19-T19)/1000</f>
+        <v>1.89743222222222</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B20" s="7" t="n">
         <v>16</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E20" s="7" t="n">
         <v>35</v>
@@ -1762,10 +1952,10 @@
         <v>1.89</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="J20" s="7" t="n">
         <v>1230</v>
@@ -1777,7 +1967,7 @@
         <v>1300</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="N20" s="7" t="n">
         <v>0.95</v>
@@ -1793,22 +1983,34 @@
         <v>25</v>
       </c>
       <c r="R20" s="7" t="n">
+        <f aca="false">K20/100</f>
+        <v>0.82</v>
+      </c>
+      <c r="S20" s="7" t="n">
         <f aca="false">Q20/18</f>
         <v>1.38888888888889</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T20" s="0" t="n">
+        <f aca="false">S20*(1-R20)</f>
+        <v>0.25</v>
+      </c>
+      <c r="U20" s="0" t="n">
+        <f aca="false">L20*(S20-T20)/1000</f>
+        <v>1.48055555555556</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B21" s="7" t="n">
         <v>17</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E21" s="7" t="n">
         <v>14</v>
@@ -1820,10 +2022,10 @@
         <v>1.63</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="J21" s="7" t="n">
         <v>1500</v>
@@ -1835,7 +2037,7 @@
         <v>1240</v>
       </c>
       <c r="M21" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="N21" s="7" t="n">
         <v>1.21</v>
@@ -1851,22 +2053,34 @@
         <v>22.7</v>
       </c>
       <c r="R21" s="7" t="n">
+        <f aca="false">K21/100</f>
+        <v>0.9</v>
+      </c>
+      <c r="S21" s="7" t="n">
         <f aca="false">Q21/18</f>
         <v>1.26111111111111</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T21" s="0" t="n">
+        <f aca="false">S21*(1-R21)</f>
+        <v>0.126111111111111</v>
+      </c>
+      <c r="U21" s="0" t="n">
+        <f aca="false">L21*(S21-T21)/1000</f>
+        <v>1.4074</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B22" s="7" t="n">
         <v>18</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E22" s="7" t="n">
         <v>46</v>
@@ -1878,10 +2092,10 @@
         <v>1.54</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="J22" s="7" t="n">
         <v>1300</v>
@@ -1893,7 +2107,7 @@
         <v>1250</v>
       </c>
       <c r="M22" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="N22" s="7" t="n">
         <v>0.84</v>
@@ -1909,22 +2123,34 @@
         <v>23.3</v>
       </c>
       <c r="R22" s="7" t="n">
+        <f aca="false">K22/100</f>
+        <v>0.86</v>
+      </c>
+      <c r="S22" s="7" t="n">
         <f aca="false">Q22/18</f>
         <v>1.29444444444444</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T22" s="0" t="n">
+        <f aca="false">S22*(1-R22)</f>
+        <v>0.181222222222222</v>
+      </c>
+      <c r="U22" s="0" t="n">
+        <f aca="false">L22*(S22-T22)/1000</f>
+        <v>1.39152777777777</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B23" s="7" t="n">
         <v>19</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E23" s="7" t="n">
         <v>32</v>
@@ -1936,10 +2162,10 @@
         <v>1.89</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="J23" s="7" t="n">
         <v>1510</v>
@@ -1951,7 +2177,7 @@
         <v>1260</v>
       </c>
       <c r="M23" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="N23" s="7" t="n">
         <v>1.2</v>
@@ -1967,22 +2193,34 @@
         <v>22.7</v>
       </c>
       <c r="R23" s="7" t="n">
+        <f aca="false">K23/100</f>
+        <v>0.9</v>
+      </c>
+      <c r="S23" s="7" t="n">
         <f aca="false">Q23/18</f>
         <v>1.26111111111111</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T23" s="0" t="n">
+        <f aca="false">S23*(1-R23)</f>
+        <v>0.126111111111111</v>
+      </c>
+      <c r="U23" s="0" t="n">
+        <f aca="false">L23*(S23-T23)/1000</f>
+        <v>1.4301</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B24" s="7" t="n">
         <v>20</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E24" s="7" t="n">
         <v>29</v>
@@ -1994,10 +2232,10 @@
         <v>1.68</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J24" s="7" t="n">
         <v>1120</v>
@@ -2009,7 +2247,7 @@
         <v>1990</v>
       </c>
       <c r="M24" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="N24" s="7" t="n">
         <v>0.56</v>
@@ -2025,22 +2263,34 @@
         <v>14.7</v>
       </c>
       <c r="R24" s="7" t="n">
+        <f aca="false">K24/100</f>
+        <v>0.91</v>
+      </c>
+      <c r="S24" s="7" t="n">
         <f aca="false">Q24/18</f>
         <v>0.816666666666667</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T24" s="0" t="n">
+        <f aca="false">S24*(1-R24)</f>
+        <v>0.0735</v>
+      </c>
+      <c r="U24" s="0" t="n">
+        <f aca="false">L24*(S24-T24)/1000</f>
+        <v>1.47890166666667</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B25" s="7" t="n">
         <v>21</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E25" s="7" t="n">
         <v>38</v>
@@ -2052,10 +2302,10 @@
         <v>1.84</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="J25" s="7" t="n">
         <v>1530</v>
@@ -2067,7 +2317,7 @@
         <v>1890</v>
       </c>
       <c r="M25" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="N25" s="7" t="n">
         <v>0.81</v>
@@ -2083,22 +2333,34 @@
         <v>21.2</v>
       </c>
       <c r="R25" s="7" t="n">
+        <f aca="false">K25/100</f>
+        <v>0.85</v>
+      </c>
+      <c r="S25" s="7" t="n">
         <f aca="false">Q25/18</f>
         <v>1.17777777777778</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T25" s="0" t="n">
+        <f aca="false">S25*(1-R25)</f>
+        <v>0.176666666666667</v>
+      </c>
+      <c r="U25" s="0" t="n">
+        <f aca="false">L25*(S25-T25)/1000</f>
+        <v>1.8921</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B26" s="7" t="n">
         <v>22</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E26" s="7" t="n">
         <v>50</v>
@@ -2110,10 +2372,10 @@
         <v>2.06</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="J26" s="7" t="n">
         <v>2500</v>
@@ -2125,7 +2387,7 @@
         <v>3100</v>
       </c>
       <c r="M26" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="N26" s="7" t="n">
         <v>0.81</v>
@@ -2141,22 +2403,34 @@
         <v>11.9</v>
       </c>
       <c r="R26" s="7" t="n">
+        <f aca="false">K26/100</f>
+        <v>0.77</v>
+      </c>
+      <c r="S26" s="7" t="n">
         <f aca="false">Q26/18</f>
         <v>0.661111111111111</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T26" s="0" t="n">
+        <f aca="false">S26*(1-R26)</f>
+        <v>0.152055555555556</v>
+      </c>
+      <c r="U26" s="0" t="n">
+        <f aca="false">L26*(S26-T26)/1000</f>
+        <v>1.57807222222222</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B27" s="7" t="n">
         <v>23</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E27" s="7" t="n">
         <v>50</v>
@@ -2168,10 +2442,10 @@
         <v>1.77</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="J27" s="7" t="n">
         <v>1370</v>
@@ -2183,7 +2457,7 @@
         <v>1000</v>
       </c>
       <c r="M27" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="N27" s="7" t="n">
         <v>1.38</v>
@@ -2199,22 +2473,34 @@
         <v>23.5</v>
       </c>
       <c r="R27" s="7" t="n">
+        <f aca="false">K27/100</f>
+        <v>0.92</v>
+      </c>
+      <c r="S27" s="7" t="n">
         <f aca="false">Q27/18</f>
         <v>1.30555555555556</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T27" s="0" t="n">
+        <f aca="false">S27*(1-R27)</f>
+        <v>0.104444444444445</v>
+      </c>
+      <c r="U27" s="0" t="n">
+        <f aca="false">L27*(S27-T27)/1000</f>
+        <v>1.20111111111112</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B28" s="7" t="n">
         <v>24</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E28" s="7" t="n">
         <v>39</v>
@@ -2226,10 +2512,10 @@
         <v>1.66</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="J28" s="7" t="n">
         <v>1080</v>
@@ -2241,7 +2527,7 @@
         <v>1450</v>
       </c>
       <c r="M28" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="N28" s="7" t="n">
         <v>0.75</v>
@@ -2257,22 +2543,34 @@
         <v>28.6</v>
       </c>
       <c r="R28" s="7" t="n">
+        <f aca="false">K28/100</f>
+        <v>0.94</v>
+      </c>
+      <c r="S28" s="7" t="n">
         <f aca="false">Q28/18</f>
         <v>1.58888888888889</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T28" s="0" t="n">
+        <f aca="false">S28*(1-R28)</f>
+        <v>0.0953333333333335</v>
+      </c>
+      <c r="U28" s="0" t="n">
+        <f aca="false">L28*(S28-T28)/1000</f>
+        <v>2.16565555555556</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B29" s="7" t="n">
         <v>25</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E29" s="7" t="n">
         <v>30</v>
@@ -2284,10 +2582,10 @@
         <v>1.71</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="J29" s="7" t="n">
         <v>1100</v>
@@ -2299,7 +2597,7 @@
         <v>1420</v>
       </c>
       <c r="M29" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="N29" s="7" t="n">
         <v>0.77</v>
@@ -2315,37 +2613,49 @@
         <v>28.2</v>
       </c>
       <c r="R29" s="7" t="n">
+        <f aca="false">K29/100</f>
+        <v>0.86</v>
+      </c>
+      <c r="S29" s="7" t="n">
         <f aca="false">Q29/18</f>
         <v>1.56666666666667</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T29" s="0" t="n">
+        <f aca="false">S29*(1-R29)</f>
+        <v>0.219333333333334</v>
+      </c>
+      <c r="U29" s="0" t="n">
+        <f aca="false">L29*(S29-T29)/1000</f>
+        <v>1.91321333333334</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B30" s="7" t="n">
         <v>26</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E30" s="7" t="n">
         <v>33</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J30" s="7" t="n">
         <v>1840</v>
@@ -2354,13 +2664,13 @@
         <v>72</v>
       </c>
       <c r="L30" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="M30" s="7" t="n">
         <v>2557</v>
       </c>
       <c r="N30" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="O30" s="7" t="n">
         <v>256</v>
@@ -2373,37 +2683,48 @@
         <v>13.9</v>
       </c>
       <c r="R30" s="7" t="n">
+        <f aca="false">K30/100</f>
+        <v>0.72</v>
+      </c>
+      <c r="S30" s="7" t="n">
         <f aca="false">Q30/18</f>
         <v>0.772222222222222</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T30" s="0" t="n">
+        <f aca="false">S30*(1-R30)</f>
+        <v>0.216222222222222</v>
+      </c>
+      <c r="U30" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B31" s="7" t="n">
         <v>27</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E31" s="7" t="n">
         <v>28</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J31" s="7" t="n">
         <v>1460</v>
@@ -2412,13 +2733,13 @@
         <v>76</v>
       </c>
       <c r="L31" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="M31" s="7" t="n">
         <v>1920</v>
       </c>
       <c r="N31" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="O31" s="7" t="n">
         <v>349</v>
@@ -2431,37 +2752,48 @@
         <v>23.9</v>
       </c>
       <c r="R31" s="7" t="n">
+        <f aca="false">K31/100</f>
+        <v>0.76</v>
+      </c>
+      <c r="S31" s="7" t="n">
         <f aca="false">Q31/18</f>
         <v>1.32777777777778</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T31" s="0" t="n">
+        <f aca="false">S31*(1-R31)</f>
+        <v>0.318666666666667</v>
+      </c>
+      <c r="U31" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B32" s="7" t="n">
         <v>28</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E32" s="7" t="n">
         <v>38</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="J32" s="7" t="n">
         <v>1550</v>
@@ -2470,13 +2802,13 @@
         <v>78</v>
       </c>
       <c r="L32" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="M32" s="7" t="n">
         <v>1990</v>
       </c>
       <c r="N32" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="O32" s="7" t="n">
         <v>204</v>
@@ -2489,37 +2821,48 @@
         <v>13.1</v>
       </c>
       <c r="R32" s="7" t="n">
+        <f aca="false">K32/100</f>
+        <v>0.78</v>
+      </c>
+      <c r="S32" s="7" t="n">
         <f aca="false">Q32/18</f>
         <v>0.727777777777778</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T32" s="0" t="n">
+        <f aca="false">S32*(1-R32)</f>
+        <v>0.160111111111111</v>
+      </c>
+      <c r="U32" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B33" s="7" t="n">
         <v>29</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E33" s="7" t="n">
         <v>43</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="J33" s="7" t="n">
         <v>1610</v>
@@ -2534,7 +2877,7 @@
         <v>2120</v>
       </c>
       <c r="N33" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="O33" s="7" t="n">
         <v>219</v>
@@ -2547,37 +2890,49 @@
         <v>13.6</v>
       </c>
       <c r="R33" s="7" t="n">
+        <f aca="false">K33/100</f>
+        <v>0.76</v>
+      </c>
+      <c r="S33" s="7" t="n">
         <f aca="false">Q33/18</f>
         <v>0.755555555555556</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T33" s="0" t="n">
+        <f aca="false">S33*(1-R33)</f>
+        <v>0.181333333333333</v>
+      </c>
+      <c r="U33" s="0" t="n">
+        <f aca="false">L33*(S33-T33)/1000</f>
+        <v>0.947466666666667</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B34" s="7" t="n">
         <v>30</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E34" s="7" t="n">
         <v>66</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="J34" s="7" t="n">
         <v>1050</v>
@@ -2592,7 +2947,7 @@
         <v>1660</v>
       </c>
       <c r="N34" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="O34" s="7" t="n">
         <v>206</v>
@@ -2605,37 +2960,49 @@
         <v>19.7</v>
       </c>
       <c r="R34" s="7" t="n">
+        <f aca="false">K34/100</f>
+        <v>0.63</v>
+      </c>
+      <c r="S34" s="7" t="n">
         <f aca="false">Q34/18</f>
         <v>1.09444444444444</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T34" s="0" t="n">
+        <f aca="false">S34*(1-R34)</f>
+        <v>0.404944444444443</v>
+      </c>
+      <c r="U34" s="0" t="n">
+        <f aca="false">L34*(S34-T34)/1000</f>
+        <v>1.19973</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B35" s="7" t="n">
         <v>31</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E35" s="7" t="n">
         <v>67</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="J35" s="7" t="n">
         <v>670</v>
@@ -2650,7 +3017,7 @@
         <v>990</v>
       </c>
       <c r="N35" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="O35" s="7" t="n">
         <v>296</v>
@@ -2663,37 +3030,49 @@
         <v>44</v>
       </c>
       <c r="R35" s="7" t="n">
+        <f aca="false">K35/100</f>
+        <v>0.68</v>
+      </c>
+      <c r="S35" s="7" t="n">
         <f aca="false">Q35/18</f>
         <v>2.44444444444444</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T35" s="0" t="n">
+        <f aca="false">S35*(1-R35)</f>
+        <v>0.782222222222221</v>
+      </c>
+      <c r="U35" s="0" t="n">
+        <f aca="false">L35*(S35-T35)/1000</f>
+        <v>1.59573333333333</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B36" s="7" t="n">
         <v>32</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E36" s="7" t="n">
         <v>57</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="H36" s="9" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="J36" s="7" t="n">
         <v>860</v>
@@ -2702,13 +3081,13 @@
         <v>57</v>
       </c>
       <c r="L36" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="M36" s="7" t="n">
         <v>1510</v>
       </c>
       <c r="N36" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="O36" s="7" t="n">
         <v>204</v>
@@ -2721,37 +3100,48 @@
         <v>23.7</v>
       </c>
       <c r="R36" s="7" t="n">
+        <f aca="false">K36/100</f>
+        <v>0.57</v>
+      </c>
+      <c r="S36" s="7" t="n">
         <f aca="false">Q36/18</f>
         <v>1.31666666666667</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T36" s="0" t="n">
+        <f aca="false">S36*(1-R36)</f>
+        <v>0.566166666666668</v>
+      </c>
+      <c r="U36" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B37" s="7" t="n">
         <v>33</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E37" s="7" t="n">
         <v>57</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="H37" s="9" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="J37" s="7" t="n">
         <v>730</v>
@@ -2766,7 +3156,7 @@
         <v>1160</v>
       </c>
       <c r="N37" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="O37" s="7" t="n">
         <v>209</v>
@@ -2779,37 +3169,49 @@
         <v>28.7</v>
       </c>
       <c r="R37" s="7" t="n">
+        <f aca="false">K37/100</f>
+        <v>0.63</v>
+      </c>
+      <c r="S37" s="7" t="n">
         <f aca="false">Q37/18</f>
         <v>1.59444444444444</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T37" s="0" t="n">
+        <f aca="false">S37*(1-R37)</f>
+        <v>0.589944444444443</v>
+      </c>
+      <c r="U37" s="0" t="n">
+        <f aca="false">L37*(S37-T37)/1000</f>
+        <v>0.582609999999998</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B38" s="7" t="n">
         <v>19</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E38" s="7" t="n">
         <v>32</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="H38" s="9" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="J38" s="7" t="n">
         <v>540</v>
@@ -2824,7 +3226,7 @@
         <v>1350</v>
       </c>
       <c r="N38" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="O38" s="7" t="n">
         <v>147</v>
@@ -2837,8 +3239,20 @@
         <v>27.3</v>
       </c>
       <c r="R38" s="7" t="n">
+        <f aca="false">K38/100</f>
+        <v>0.39</v>
+      </c>
+      <c r="S38" s="7" t="n">
         <f aca="false">Q38/18</f>
         <v>1.51666666666667</v>
+      </c>
+      <c r="T38" s="0" t="n">
+        <f aca="false">S38*(1-R38)</f>
+        <v>0.925166666666669</v>
+      </c>
+      <c r="U38" s="0" t="n">
+        <f aca="false">L38*(S38-T38)/1000</f>
+        <v>0.632905000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>